<commit_message>
Working model with consolidation of some components.
</commit_message>
<xml_diff>
--- a/Feed_Force_Calcs/Feed Force Calc.xlsx
+++ b/Feed_Force_Calcs/Feed Force Calc.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault.sharepoint.com/sites/Team2-Droneassistedconstructionlayoutcopy/Shared Documents/Avengers Assemble!/TA-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knech\OneDrive\Documents\ASE6002\ModelProject\Feed_Force_Calcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="11_438F0EA5382234719EA753803BE52E373CED4083" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF5FEAD3-9519-404C-98A7-1777822C8A2B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37F8735-DAEE-4811-9F66-05031CCF8A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28140" yWindow="2790" windowWidth="19260" windowHeight="15825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="Avg_Lift_Force">Sheet1!$M$4</definedName>
     <definedName name="Bar_Length">Sheet1!$B$2</definedName>
     <definedName name="Feed_Force">Sheet1!$G$2</definedName>
     <definedName name="Grip_Length">Sheet1!$B$3</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Inputs</t>
   </si>
@@ -71,9 +72,6 @@
     <t>Grip Length</t>
   </si>
   <si>
-    <t>Total Weight</t>
-  </si>
-  <si>
     <t>Avg Lift Force</t>
   </si>
   <si>
@@ -86,16 +84,7 @@
     <t>N</t>
   </si>
   <si>
-    <t>Total Weight Force</t>
-  </si>
-  <si>
     <t>Balance Lift</t>
-  </si>
-  <si>
-    <t>Feed Force, Balance</t>
-  </si>
-  <si>
-    <t>Additional Force Applied</t>
   </si>
 </sst>
 </file>
@@ -105,7 +94,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,18 +523,18 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -570,8 +559,8 @@
         <v>5</v>
       </c>
       <c r="G2" s="2">
-        <f>M8+M9</f>
-        <v>57.226017460099996</v>
+        <f>M7</f>
+        <v>45.371860476059993</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
@@ -584,7 +573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -602,82 +591,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="L4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4">
-        <v>7.5</v>
-      </c>
-      <c r="L4" t="s">
-        <v>10</v>
       </c>
       <c r="M4">
         <v>17</v>
       </c>
       <c r="N4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M5" s="2">
         <f>M4*4.4482216153</f>
         <v>75.619767460099993</v>
       </c>
       <c r="N5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="L7" t="s">
         <v>13</v>
       </c>
+      <c r="M7" s="2">
+        <f>(M5*M3)/(M2)</f>
+        <v>45.371860476059993</v>
+      </c>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="L6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="2">
-        <f>B4*9.81</f>
-        <v>73.575000000000003</v>
-      </c>
-      <c r="N6" t="s">
-        <v>13</v>
-      </c>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M8" s="2"/>
     </row>
-    <row r="7" spans="1:15">
-      <c r="L7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M7" s="2">
-        <f>(M6*M2)/(M2+M3)</f>
-        <v>45.984375</v>
-      </c>
-      <c r="N7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="L8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="2">
-        <f>M6-M7</f>
-        <v>27.590625000000003</v>
-      </c>
-      <c r="N8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="L9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="2">
-        <f>M5-M7</f>
-        <v>29.635392460099993</v>
-      </c>
-      <c r="N9" t="s">
-        <v>13</v>
-      </c>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M9" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -848,13 +804,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{288879D3-6B17-4F49-9E89-8CB8FC2F4954}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{288879D3-6B17-4F49-9E89-8CB8FC2F4954}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FD4F8D5-9EBF-489F-904D-7CF4B20C62C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FD4F8D5-9EBF-489F-904D-7CF4B20C62C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D88F03BB-698D-42DE-8ED2-671942D9E283}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D88F03BB-698D-42DE-8ED2-671942D9E283}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2de6f903-a70b-4d4e-9d47-d88418a90129"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>